<commit_message>
Issue #33 - Fixed
</commit_message>
<xml_diff>
--- a/Resources/1-issue-33-test-data-results.xlsx
+++ b/Resources/1-issue-33-test-data-results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="170">
   <si>
     <t>Order type</t>
   </si>
@@ -479,6 +479,54 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>3014010588</t>
+  </si>
+  <si>
+    <t>1CO Created</t>
+  </si>
+  <si>
+    <t>3014010589</t>
+  </si>
+  <si>
+    <t>2CO Created</t>
+  </si>
+  <si>
+    <t>3014010590</t>
+  </si>
+  <si>
+    <t>3CO Created</t>
+  </si>
+  <si>
+    <t>3014010591</t>
+  </si>
+  <si>
+    <t>4CO Created</t>
+  </si>
+  <si>
+    <t>3014010592</t>
+  </si>
+  <si>
+    <t>5CO Created</t>
+  </si>
+  <si>
+    <t>3014010593</t>
+  </si>
+  <si>
+    <t>6CO Created</t>
+  </si>
+  <si>
+    <t>3014010594</t>
+  </si>
+  <si>
+    <t>7CO Created</t>
+  </si>
+  <si>
+    <t>3014010595</t>
+  </si>
+  <si>
+    <t>8CO Created</t>
   </si>
 </sst>
 </file>
@@ -694,13 +742,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -717,13 +765,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -740,13 +788,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -763,13 +811,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -786,13 +834,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -809,13 +857,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -848,7 +896,7 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4" tint="0.49995422223578601"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1373,12 +1421,12 @@
   <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="3" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -1497,6 +1545,12 @@
       </c>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="C2" s="4" t="s">
         <v>146</v>
       </c>
@@ -1529,6 +1583,12 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="C3" t="s">
         <v>148</v>
       </c>
@@ -1561,6 +1621,12 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>148</v>
       </c>
@@ -1593,6 +1659,12 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>148</v>
       </c>
@@ -1625,6 +1697,12 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>148</v>
       </c>
@@ -1657,6 +1735,12 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>148</v>
       </c>
@@ -1689,6 +1773,12 @@
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>148</v>
       </c>
@@ -1721,6 +1811,12 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>148</v>
       </c>

</xml_diff>